<commit_message>
Fixes sort part 1
</commit_message>
<xml_diff>
--- a/trasn_cost.xlsx
+++ b/trasn_cost.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python Repo\Streamlit app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{65DD9179-F567-44B0-9A66-645B774FCFB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5028B9-051A-4D8C-882A-EE0E36506EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="2124" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Καιμακλί</t>
   </si>
   <si>
-    <t>Eγκωμη</t>
-  </si>
-  <si>
     <t>Ακάκι</t>
   </si>
   <si>
@@ -358,12 +355,15 @@
   </si>
   <si>
     <t>Agaia Marina Xrusoxous</t>
+  </si>
+  <si>
+    <t>Εγκωμη</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -708,11 +708,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,181 +779,181 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>64</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>65</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>66</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>72</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>74</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>90</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>91</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>92</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>93</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>94</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>95</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>96</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>97</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>98</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>99</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>100</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>101</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>102</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>103</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>104</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>105</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>106</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>107</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>108</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>109</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
@@ -1495,7 +1495,7 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>17</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>33</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -4180,7 +4180,7 @@
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -4538,7 +4538,7 @@
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>7</v>
@@ -5254,7 +5254,7 @@
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>58</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>66</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>67</v>
@@ -5791,7 +5791,7 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>60</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>62</v>
@@ -6149,7 +6149,7 @@
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>32</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>29</v>
@@ -6507,7 +6507,7 @@
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>37</v>
@@ -6686,7 +6686,7 @@
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34">
         <v>22</v>
@@ -6865,7 +6865,7 @@
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35">
         <v>37</v>
@@ -7044,7 +7044,7 @@
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>30</v>
@@ -7223,7 +7223,7 @@
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>23</v>
@@ -7402,7 +7402,7 @@
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>33</v>
@@ -7581,7 +7581,7 @@
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39">
         <v>48</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -7939,7 +7939,7 @@
     </row>
     <row r="41" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41">
         <v>38</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>60</v>
@@ -8297,7 +8297,7 @@
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>49</v>
@@ -8476,7 +8476,7 @@
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>53</v>
@@ -8655,7 +8655,7 @@
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>56</v>
@@ -8834,7 +8834,7 @@
     </row>
     <row r="46" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>58</v>
@@ -9013,7 +9013,7 @@
     </row>
     <row r="47" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>102</v>
@@ -9192,7 +9192,7 @@
     </row>
     <row r="48" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48">
         <v>94</v>
@@ -9371,7 +9371,7 @@
     </row>
     <row r="49" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>103</v>
@@ -9550,7 +9550,7 @@
     </row>
     <row r="50" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>111</v>
@@ -9729,7 +9729,7 @@
     </row>
     <row r="51" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>132</v>
@@ -9908,7 +9908,7 @@
     </row>
     <row r="52" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52">
         <v>123</v>
@@ -10087,7 +10087,7 @@
     </row>
     <row r="53" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53">
         <v>106</v>

</xml_diff>

<commit_message>
Fixes sort part 2 - capitalization
</commit_message>
<xml_diff>
--- a/trasn_cost.xlsx
+++ b/trasn_cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python Repo\Streamlit app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5028B9-051A-4D8C-882A-EE0E36506EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2D83BA-B651-4178-ADB6-F5E5D183EA68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="3096" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,184 +180,184 @@
     <t>Αγ. Μαρίνα Χρυσ.</t>
   </si>
   <si>
-    <t>Makareio</t>
-  </si>
-  <si>
-    <t>Neo GSP</t>
-  </si>
-  <si>
-    <t>Aglantzia</t>
-  </si>
-  <si>
-    <t>Latsia</t>
-  </si>
-  <si>
-    <t>Ergates</t>
-  </si>
-  <si>
-    <t>Anageia</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Nisou</t>
-  </si>
-  <si>
-    <t>Dali</t>
-  </si>
-  <si>
-    <t>Lympia</t>
-  </si>
-  <si>
-    <t>Kokkinotrimithia</t>
-  </si>
-  <si>
-    <t>Paliometoxo</t>
-  </si>
-  <si>
-    <t>Mammari</t>
-  </si>
-  <si>
-    <t>Peristerona</t>
-  </si>
-  <si>
-    <t>Lakatameia</t>
-  </si>
-  <si>
-    <t>Kotsiatis</t>
-  </si>
-  <si>
-    <t>Lythrodontas</t>
-  </si>
-  <si>
-    <t>Korakou</t>
-  </si>
-  <si>
-    <t>Kuperounta</t>
-  </si>
-  <si>
-    <t>Pelendri</t>
-  </si>
-  <si>
-    <t>Lemesos</t>
-  </si>
-  <si>
-    <t>Polemidia</t>
-  </si>
-  <si>
-    <t>Zakaki</t>
-  </si>
-  <si>
-    <t>Pareklisia</t>
-  </si>
-  <si>
-    <t>Germasogeia</t>
-  </si>
-  <si>
-    <t>Kolossi</t>
-  </si>
-  <si>
-    <t>Traxoni</t>
-  </si>
-  <si>
-    <t>Erimi</t>
-  </si>
-  <si>
-    <t>Ypsonas</t>
-  </si>
-  <si>
-    <t>Akrotiti</t>
-  </si>
-  <si>
-    <t>Larnaca</t>
-  </si>
-  <si>
-    <t>Aradippou</t>
-  </si>
-  <si>
-    <t>Agios Theodoros Larnaca</t>
-  </si>
-  <si>
-    <t>Psevdas</t>
-  </si>
-  <si>
-    <t>Oroklini</t>
-  </si>
-  <si>
-    <t>Pula</t>
-  </si>
-  <si>
-    <t>Kornos</t>
-  </si>
-  <si>
-    <t>Athienou</t>
-  </si>
-  <si>
-    <t>Leivadia</t>
-  </si>
-  <si>
-    <t>Troulloi</t>
-  </si>
-  <si>
-    <t>Kiti</t>
-  </si>
-  <si>
-    <t>Ormideia</t>
-  </si>
-  <si>
-    <t>Lefkara</t>
-  </si>
-  <si>
-    <t>Xulofagou</t>
-  </si>
-  <si>
-    <t>Xulotumpou</t>
-  </si>
-  <si>
-    <t>Dasaki Axnas</t>
-  </si>
-  <si>
-    <t>Agia Napa</t>
-  </si>
-  <si>
-    <t>Deruneia</t>
-  </si>
-  <si>
-    <t>Paralimni</t>
-  </si>
-  <si>
-    <t>Avgorou</t>
-  </si>
-  <si>
-    <t>Liopetri</t>
-  </si>
-  <si>
-    <t>Frenaros</t>
-  </si>
-  <si>
-    <t>Sotira</t>
-  </si>
-  <si>
-    <t>Pafos</t>
-  </si>
-  <si>
-    <t>Xloraka</t>
-  </si>
-  <si>
-    <t>Pegeia</t>
-  </si>
-  <si>
-    <t>Geroskupou</t>
-  </si>
-  <si>
-    <t>Polis Xrisoxous</t>
-  </si>
-  <si>
-    <t>Agaia Marina Xrusoxous</t>
-  </si>
-  <si>
     <t>Εγκωμη</t>
+  </si>
+  <si>
+    <t>ΜΑΚΑΡΙΟ</t>
+  </si>
+  <si>
+    <t>ΝΕΟ ΓΣΠ</t>
+  </si>
+  <si>
+    <t>ΑΓΛΑΝΤΖΙΑ</t>
+  </si>
+  <si>
+    <t>ΛΑΤΣΙΑ</t>
+  </si>
+  <si>
+    <t>ΕΡΓΑΤΕΣ</t>
+  </si>
+  <si>
+    <t>ΑΝΑΓΥΙΑ</t>
+  </si>
+  <si>
+    <t>ΝΗΣΟΥ</t>
+  </si>
+  <si>
+    <t>ΔΑΛΙ</t>
+  </si>
+  <si>
+    <t>ΛΥΜΠΙΑ</t>
+  </si>
+  <si>
+    <t>ΚΟΚΚΙΝΟΤΡΙΜΙΘΙΑ</t>
+  </si>
+  <si>
+    <t>ΠΑΛΙΟΜΕΤΟΧΟ</t>
+  </si>
+  <si>
+    <t>ΜΑΜΜΑΡΙ</t>
+  </si>
+  <si>
+    <t>ΠΕΡΙΣΤΕΡΩΝΑ</t>
+  </si>
+  <si>
+    <t>ΛΑΚΑΤΑΜΕΙΑ</t>
+  </si>
+  <si>
+    <t>ΚΟΤΣΙΑΤΗΣ</t>
+  </si>
+  <si>
+    <t>ΛΥΘΡΟΔΟΝΤΑΣ</t>
+  </si>
+  <si>
+    <t>ΚΟΡΑΚΟΥ</t>
+  </si>
+  <si>
+    <t>ΚΥΠΕΡΟΥΝΤΑ</t>
+  </si>
+  <si>
+    <t>ΠΕΛΕΝΔΡΙ</t>
+  </si>
+  <si>
+    <t>ΛΕΜΕΣΟΣ</t>
+  </si>
+  <si>
+    <t>ΠΟΛΕΜΙΔΙΑ</t>
+  </si>
+  <si>
+    <t>ΖΑΚΑΚΙ</t>
+  </si>
+  <si>
+    <t>ΠΑΡΕΚΚΛΗΣΣΙΑ</t>
+  </si>
+  <si>
+    <t>ΚΟΛΟΣΣΙ</t>
+  </si>
+  <si>
+    <t>ΤΡΑΧΩΝΙ</t>
+  </si>
+  <si>
+    <t>ΕΡΗΜΗ</t>
+  </si>
+  <si>
+    <t>ΑΚΡΩΤΗΡΙ</t>
+  </si>
+  <si>
+    <t>ΓΕΡΜΑΣΟΓΕΙΑ</t>
+  </si>
+  <si>
+    <t>ΎΨΩΝΑΣ</t>
+  </si>
+  <si>
+    <t>ΛΑΡΝΑΚΑ</t>
+  </si>
+  <si>
+    <t>ΑΡΑΔΙΠΠΟΥ</t>
+  </si>
+  <si>
+    <t>ΑΓ. ΘΕΟΔΩΡΟΣ Λ/ΚΑΣ</t>
+  </si>
+  <si>
+    <t>ΨΕΥΔΑΣ</t>
+  </si>
+  <si>
+    <t>ΟΡΟΚΛΙΝΗ</t>
+  </si>
+  <si>
+    <t>ΠΥΛΑ</t>
+  </si>
+  <si>
+    <t>ΚΟΡΝΟΣ</t>
+  </si>
+  <si>
+    <t>ΑΘΗΑΙΝΟΥ</t>
+  </si>
+  <si>
+    <t>ΛΕΙΒΑΔΙΑ</t>
+  </si>
+  <si>
+    <t>ΤΡΟΥΛΛΟΙ</t>
+  </si>
+  <si>
+    <t>ΚΙΤΙ</t>
+  </si>
+  <si>
+    <t>ΟΡΜΗΔΕΙΑ</t>
+  </si>
+  <si>
+    <t>ΛΕΥΚΑΡΑ</t>
+  </si>
+  <si>
+    <t>ΞΥΛΟΦΑΓΟΥ</t>
+  </si>
+  <si>
+    <t>ΥΛΟΤΥΜΠΟΥ</t>
+  </si>
+  <si>
+    <t>ΔΑΣΑΚΙ ΑΧΝΑΣ</t>
+  </si>
+  <si>
+    <t>ΑΓΙΑ ΝΑΠΑ</t>
+  </si>
+  <si>
+    <t>ΔΕΡΥΝΕΙΑ</t>
+  </si>
+  <si>
+    <t>ΠΑΡΑΛΙΜΝΙ</t>
+  </si>
+  <si>
+    <t>ΑΥΓΟΡΟΥ</t>
+  </si>
+  <si>
+    <t>ΛΙΟΠΕΤΡΙ</t>
+  </si>
+  <si>
+    <t>ΦΡΕΝΑΡΟΣ</t>
+  </si>
+  <si>
+    <t>ΣΩΤΗΡΑ</t>
+  </si>
+  <si>
+    <t>ΠΑΦΟΣ</t>
+  </si>
+  <si>
+    <t>ΧΛΩΡΑΚΑ</t>
+  </si>
+  <si>
+    <t>ΠΕΓΕΙΑ</t>
+  </si>
+  <si>
+    <t>ΓΕΡΟΣΚΗΠΟΥ</t>
+  </si>
+  <si>
+    <t>ΠΟΛΗΣ ΧΡΥΣΟΧΟΥΣ</t>
+  </si>
+  <si>
+    <t>ΑΓ. ΜΑΡΙΝΑ ΧΡΥΣΟΧΟΥΣ</t>
   </si>
 </sst>
 </file>
@@ -712,7 +712,7 @@
   <dimension ref="A1:BG53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B1" sqref="B1:BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,181 +779,181 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="V1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="X1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Y1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AC1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AD1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AF1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AG1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AH1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AI1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AJ1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AK1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AL1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AM1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AN1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AO1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AP1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AQ1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AR1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AS1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AT1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AU1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AV1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AW1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AX1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AY1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AZ1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BA1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="BB1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="BC1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="BD1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BE1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BF1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BG1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
@@ -1495,7 +1495,7 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
Fixes sort part 3 - capitalization
</commit_message>
<xml_diff>
--- a/trasn_cost.xlsx
+++ b/trasn_cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python Repo\Streamlit app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E335EB17-83A5-48BE-8AE4-A82C72431B3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E92A5F2-F29B-42ED-A099-831041485E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,9 +249,6 @@
     <t>ΑΛΑΣΣΑ</t>
   </si>
   <si>
-    <t>ΑΓ. ΙΩΑΝΝΗΣ</t>
-  </si>
-  <si>
     <t>ΥΨΩΝΑΣ</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>City</t>
+  </si>
+  <si>
+    <t>ΑΓ. ΙΩΑΝΝΗΣ Λ/ΣΟΣ</t>
   </si>
 </sst>
 </file>
@@ -636,7 +636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -702,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5714,7 +5716,7 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B29">
         <v>60</v>
@@ -5893,7 +5895,7 @@
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30">
         <v>62</v>
@@ -6788,7 +6790,7 @@
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35">
         <v>37</v>
@@ -6967,7 +6969,7 @@
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36">
         <v>30</v>
@@ -7325,7 +7327,7 @@
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38">
         <v>33</v>
@@ -7683,7 +7685,7 @@
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -9115,7 +9117,7 @@
     </row>
     <row r="48" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48">
         <v>94</v>
@@ -9294,7 +9296,7 @@
     </row>
     <row r="49" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49">
         <v>103</v>
@@ -9652,7 +9654,7 @@
     </row>
     <row r="51" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B51">
         <v>132</v>
@@ -9831,7 +9833,7 @@
     </row>
     <row r="52" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52">
         <v>123</v>
@@ -10010,7 +10012,7 @@
     </row>
     <row r="53" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53">
         <v>106</v>

</xml_diff>